<commit_message>
Consideración de la masa de entrepiso
Además también se llevó a una función la fracción de código que dibuja la numeración de la estructura
</commit_message>
<xml_diff>
--- a/avances_semanales/fase2/entrada.xlsx
+++ b/avances_semanales/fase2/entrada.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\esteb\Documents\GitHub\analisis_vibraciones\avances_semanales\fase1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\esteb\Documents\GitHub\analisis_vibraciones\avances_semanales\fase2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7B24DC9-2AB2-4FCD-AD42-51A3919140C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{713E6A79-6CFC-485A-91FD-2836CBD3D588}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="xy_nod" sheetId="1" r:id="rId1"/>
@@ -85,6 +85,58 @@
     <author>Esteban Hernández Soto</author>
   </authors>
   <commentList>
+    <comment ref="G1" authorId="0" shapeId="0" xr:uid="{3D411952-ABF1-40A2-8F36-A4AF6B517804}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>para elementos que reciben la masa de las losas, si no aplica dejar en blanco</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H1" authorId="0" shapeId="0" xr:uid="{CAEC1589-8AB9-4002-BB97-DB2DF091BEE5}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>para elementos de entrepiso, si no aplica dejar en blanco</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I1" authorId="0" shapeId="0" xr:uid="{F29E21AA-9DE0-4CE1-9D0D-8555BBC89A49}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>si no aplica dejar en blanco</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Esteban Hernández Soto</author>
+  </authors>
+  <commentList>
     <comment ref="B1" authorId="0" shapeId="0" xr:uid="{004D5AB9-399F-4527-9086-EE1CE8699D45}">
       <text>
         <r>
@@ -115,7 +167,7 @@
 </comments>
 </file>
 
-<file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Esteban Hernández Soto</author>
@@ -191,7 +243,7 @@
 </comments>
 </file>
 
-<file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/comments5.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Esteban Hernández Soto</author>
@@ -251,7 +303,7 @@
 </comments>
 </file>
 
-<file path=xl/comments5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/comments6.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Esteban Hernández Soto</author>
@@ -357,7 +409,7 @@
 </comments>
 </file>
 
-<file path=xl/comments6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/comments7.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Esteban Hernández Soto</author>
@@ -424,7 +476,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="24">
   <si>
     <t>x</t>
   </si>
@@ -487,6 +539,15 @@
   </si>
   <si>
     <t>q2</t>
+  </si>
+  <si>
+    <t>Af</t>
+  </si>
+  <si>
+    <t>espesor</t>
+  </si>
+  <si>
+    <t>material_losa</t>
   </si>
 </sst>
 </file>
@@ -622,13 +683,14 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="3"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="3" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="2" applyFont="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="20% - Accent2" xfId="3" builtinId="34"/>
@@ -637,11 +699,6 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="7">
-    <dxf>
-      <font>
-        <b val="0"/>
-      </font>
-    </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
@@ -685,6 +742,11 @@
         <b val="0"/>
       </font>
     </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+      </font>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -715,29 +777,35 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{39D54B7D-B2CA-418B-9C9E-25DFCF61B9BE}" name="Table2" displayName="Table2" ref="A1:F43" totalsRowShown="0" headerRowDxfId="0" headerRowCellStyle="Accent2" dataCellStyle="Input">
-  <autoFilter ref="A1:F43" xr:uid="{39D54B7D-B2CA-418B-9C9E-25DFCF61B9BE}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{39D54B7D-B2CA-418B-9C9E-25DFCF61B9BE}" name="Table2" displayName="Table2" ref="A1:I43" totalsRowShown="0" headerRowDxfId="5" headerRowCellStyle="Accent2" dataCellStyle="Input">
+  <autoFilter ref="A1:I43" xr:uid="{39D54B7D-B2CA-418B-9C9E-25DFCF61B9BE}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
     <filterColumn colId="3" hiddenButton="1"/>
     <filterColumn colId="4" hiddenButton="1"/>
     <filterColumn colId="5" hiddenButton="1"/>
+    <filterColumn colId="6" hiddenButton="1"/>
+    <filterColumn colId="7" hiddenButton="1"/>
+    <filterColumn colId="8" hiddenButton="1"/>
   </autoFilter>
-  <tableColumns count="6">
+  <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{65B86E80-94EE-4957-906D-C9FB9A847C3D}" name="elemento" dataCellStyle="20% - Accent2"/>
     <tableColumn id="2" xr3:uid="{2AE0CE3E-EB68-4993-BFC0-A1FC728D0098}" name="NL1" dataCellStyle="Input"/>
     <tableColumn id="3" xr3:uid="{1A5A9640-CD9E-44AD-BD3A-D954B370202F}" name="NL2" dataCellStyle="Input"/>
     <tableColumn id="4" xr3:uid="{16D47387-1CCF-4D3A-9E7A-D126820761D6}" name="material" dataCellStyle="Input"/>
     <tableColumn id="6" xr3:uid="{7C48F9C3-42CB-4786-B2EE-FCA0D5AE3FFD}" name="seccion" dataCellStyle="Input"/>
     <tableColumn id="5" xr3:uid="{34ACEC23-7B35-4421-8A35-FA55EEFFF0FB}" name="tipo" dataCellStyle="Input"/>
+    <tableColumn id="7" xr3:uid="{E16E8D08-B034-4924-9C03-37BC653871CC}" name="Af" dataCellStyle="Input"/>
+    <tableColumn id="8" xr3:uid="{C05D044A-C969-4B69-8B4C-D3005BF0CFC5}" name="espesor" dataCellStyle="Input"/>
+    <tableColumn id="9" xr3:uid="{A820069D-FFC9-4F6E-A14A-78A7E6E3331F}" name="material_losa" dataCellStyle="Input"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight10" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{42A1F5DA-D51B-45C6-8DA0-76544453A939}" name="Table3" displayName="Table3" ref="A1:C13" totalsRowShown="0" tableBorderDxfId="5" headerRowCellStyle="Accent2" dataCellStyle="Input">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{42A1F5DA-D51B-45C6-8DA0-76544453A939}" name="Table3" displayName="Table3" ref="A1:C13" totalsRowShown="0" tableBorderDxfId="4" headerRowCellStyle="Accent2" dataCellStyle="Input">
   <autoFilter ref="A1:C13" xr:uid="{42A1F5DA-D51B-45C6-8DA0-76544453A939}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -762,7 +830,7 @@
     <filterColumn colId="4" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{880723F3-A638-4CBF-99AF-D7262FD3C8A9}" name="elemento" dataDxfId="4" dataCellStyle="Input">
+    <tableColumn id="1" xr3:uid="{880723F3-A638-4CBF-99AF-D7262FD3C8A9}" name="elemento" dataDxfId="3" dataCellStyle="Input">
       <calculatedColumnFormula>Table2[[#This Row],[elemento]]</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="2" xr3:uid="{578B6873-02F7-4B1D-BC80-1523396AF35F}" name="b1" dataCellStyle="Input"/>
@@ -775,7 +843,7 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{9628A17C-93B8-489C-A49F-43E1D314D611}" name="Table5" displayName="Table5" ref="A1:C7" totalsRowShown="0" tableBorderDxfId="3" headerRowCellStyle="Accent2" dataCellStyle="Input">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{9628A17C-93B8-489C-A49F-43E1D314D611}" name="Table5" displayName="Table5" ref="A1:C7" totalsRowShown="0" tableBorderDxfId="2" headerRowCellStyle="Accent2" dataCellStyle="Input">
   <autoFilter ref="A1:C7" xr:uid="{9628A17C-93B8-489C-A49F-43E1D314D611}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -791,7 +859,7 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{96CDDC17-92E8-4C39-B9D1-92DA6FC81046}" name="Table6" displayName="Table6" ref="A1:C3" totalsRowShown="0" headerRowDxfId="2" headerRowCellStyle="Accent2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{96CDDC17-92E8-4C39-B9D1-92DA6FC81046}" name="Table6" displayName="Table6" ref="A1:C3" totalsRowShown="0" headerRowDxfId="1" headerRowCellStyle="Accent2">
   <autoFilter ref="A1:C3" xr:uid="{96CDDC17-92E8-4C39-B9D1-92DA6FC81046}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -815,7 +883,7 @@
   </autoFilter>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{CBB86DB4-091A-4E50-B78A-CE5FA21BDAFD}" name="seccion" dataCellStyle="20% - Accent2"/>
-    <tableColumn id="2" xr3:uid="{79326CC9-9A90-4BFE-99B8-9937ABA40CB9}" name="A" dataDxfId="1" dataCellStyle="Input">
+    <tableColumn id="2" xr3:uid="{79326CC9-9A90-4BFE-99B8-9937ABA40CB9}" name="A" dataDxfId="0" dataCellStyle="Input">
       <calculatedColumnFormula>0.3*0.5</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="3" xr3:uid="{CCC256CD-37B8-4882-BDB5-A78B019F997E}" name="I" dataCellStyle="Input">
@@ -1427,11 +1495,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6411D8F9-1C02-43E4-B965-2ED18DE2C766}">
-  <dimension ref="A1:F43"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6411D8F9-1C02-43E4-B965-2ED18DE2C766}">
+  <dimension ref="A1:I43"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="K32" sqref="K32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1440,7 +1508,7 @@
     <col min="4" max="5" width="10.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
@@ -1459,8 +1527,17 @@
       <c r="F1" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G1" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="I1" s="6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -1479,8 +1556,11 @@
       <c r="F2" s="3" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
+      <c r="I2" s="3"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -1499,8 +1579,11 @@
       <c r="F3" s="3" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G3" s="3"/>
+      <c r="H3" s="3"/>
+      <c r="I3" s="3"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -1519,8 +1602,11 @@
       <c r="F4" s="3" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G4" s="3"/>
+      <c r="H4" s="3"/>
+      <c r="I4" s="3"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -1539,8 +1625,11 @@
       <c r="F5" s="3" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G5" s="3"/>
+      <c r="H5" s="3"/>
+      <c r="I5" s="3"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -1559,8 +1648,11 @@
       <c r="F6" s="3" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G6" s="3"/>
+      <c r="H6" s="3"/>
+      <c r="I6" s="3"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -1579,8 +1671,11 @@
       <c r="F7" s="3" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G7" s="3"/>
+      <c r="H7" s="3"/>
+      <c r="I7" s="3"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -1601,8 +1696,11 @@
       <c r="F8" s="3" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G8" s="3"/>
+      <c r="H8" s="3"/>
+      <c r="I8" s="3"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -1623,8 +1721,11 @@
       <c r="F9" s="3" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G9" s="3"/>
+      <c r="H9" s="3"/>
+      <c r="I9" s="3"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>9</v>
       </c>
@@ -1645,8 +1746,11 @@
       <c r="F10" s="3" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G10" s="3"/>
+      <c r="H10" s="3"/>
+      <c r="I10" s="3"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>10</v>
       </c>
@@ -1667,8 +1771,11 @@
       <c r="F11" s="3" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G11" s="3"/>
+      <c r="H11" s="3"/>
+      <c r="I11" s="3"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>11</v>
       </c>
@@ -1689,8 +1796,11 @@
       <c r="F12" s="3" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G12" s="3"/>
+      <c r="H12" s="3"/>
+      <c r="I12" s="3"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>12</v>
       </c>
@@ -1711,8 +1821,11 @@
       <c r="F13" s="3" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G13" s="3"/>
+      <c r="H13" s="3"/>
+      <c r="I13" s="3"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>13</v>
       </c>
@@ -1733,8 +1846,11 @@
       <c r="F14" s="3" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G14" s="3"/>
+      <c r="H14" s="3"/>
+      <c r="I14" s="3"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>14</v>
       </c>
@@ -1755,8 +1871,11 @@
       <c r="F15" s="3" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G15" s="3"/>
+      <c r="H15" s="3"/>
+      <c r="I15" s="3"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>15</v>
       </c>
@@ -1777,8 +1896,11 @@
       <c r="F16" s="3" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G16" s="3"/>
+      <c r="H16" s="3"/>
+      <c r="I16" s="3"/>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>16</v>
       </c>
@@ -1799,8 +1921,11 @@
       <c r="F17" s="3" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G17" s="3"/>
+      <c r="H17" s="3"/>
+      <c r="I17" s="3"/>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <v>17</v>
       </c>
@@ -1821,8 +1946,11 @@
       <c r="F18" s="3" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G18" s="3"/>
+      <c r="H18" s="3"/>
+      <c r="I18" s="3"/>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
         <v>18</v>
       </c>
@@ -1843,8 +1971,11 @@
       <c r="F19" s="3" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G19" s="3"/>
+      <c r="H19" s="3"/>
+      <c r="I19" s="3"/>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
         <v>19</v>
       </c>
@@ -1865,8 +1996,11 @@
       <c r="F20" s="3" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G20" s="3"/>
+      <c r="H20" s="3"/>
+      <c r="I20" s="3"/>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
         <v>20</v>
       </c>
@@ -1887,8 +2021,11 @@
       <c r="F21" s="3" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G21" s="3"/>
+      <c r="H21" s="3"/>
+      <c r="I21" s="3"/>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
         <v>21</v>
       </c>
@@ -1909,8 +2046,11 @@
       <c r="F22" s="3" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G22" s="3"/>
+      <c r="H22" s="3"/>
+      <c r="I22" s="3"/>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
         <v>22</v>
       </c>
@@ -1931,8 +2071,11 @@
       <c r="F23" s="3" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G23" s="3"/>
+      <c r="H23" s="3"/>
+      <c r="I23" s="3"/>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
         <v>23</v>
       </c>
@@ -1953,8 +2096,11 @@
       <c r="F24" s="3" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G24" s="3"/>
+      <c r="H24" s="3"/>
+      <c r="I24" s="3"/>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
         <v>24</v>
       </c>
@@ -1975,8 +2121,11 @@
       <c r="F25" s="3" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G25" s="3"/>
+      <c r="H25" s="3"/>
+      <c r="I25" s="3"/>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
         <v>25</v>
       </c>
@@ -1995,8 +2144,17 @@
       <c r="F26" s="3" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G26" s="3">
+        <v>4.5</v>
+      </c>
+      <c r="H26" s="3">
+        <v>0.125</v>
+      </c>
+      <c r="I26" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
         <v>26</v>
       </c>
@@ -2015,8 +2173,17 @@
       <c r="F27" s="3" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G27" s="3">
+        <v>4.5</v>
+      </c>
+      <c r="H27" s="3">
+        <v>0.125</v>
+      </c>
+      <c r="I27" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="2">
         <v>27</v>
       </c>
@@ -2035,8 +2202,17 @@
       <c r="F28" s="3" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G28" s="3">
+        <v>4.5</v>
+      </c>
+      <c r="H28" s="3">
+        <v>0.125</v>
+      </c>
+      <c r="I28" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="2">
         <v>28</v>
       </c>
@@ -2055,8 +2231,17 @@
       <c r="F29" s="3" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G29" s="3">
+        <v>4.5</v>
+      </c>
+      <c r="H29" s="3">
+        <v>0.125</v>
+      </c>
+      <c r="I29" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="2">
         <v>29</v>
       </c>
@@ -2075,8 +2260,17 @@
       <c r="F30" s="3" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G30" s="3">
+        <v>4.5</v>
+      </c>
+      <c r="H30" s="3">
+        <v>0.125</v>
+      </c>
+      <c r="I30" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" s="2">
         <v>30</v>
       </c>
@@ -2095,8 +2289,17 @@
       <c r="F31" s="3" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G31" s="3">
+        <v>4.5</v>
+      </c>
+      <c r="H31" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="I31" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" s="2">
         <v>31</v>
       </c>
@@ -2115,8 +2318,17 @@
       <c r="F32" s="3" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G32" s="3">
+        <v>4.5</v>
+      </c>
+      <c r="H32" s="3">
+        <v>0.125</v>
+      </c>
+      <c r="I32" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="2">
         <v>32</v>
       </c>
@@ -2135,8 +2347,17 @@
       <c r="F33" s="3" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G33" s="3">
+        <v>4.5</v>
+      </c>
+      <c r="H33" s="3">
+        <v>0.125</v>
+      </c>
+      <c r="I33" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" s="2">
         <v>33</v>
       </c>
@@ -2155,8 +2376,17 @@
       <c r="F34" s="3" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G34" s="3">
+        <v>4.5</v>
+      </c>
+      <c r="H34" s="3">
+        <v>0.125</v>
+      </c>
+      <c r="I34" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" s="2">
         <v>34</v>
       </c>
@@ -2175,8 +2405,17 @@
       <c r="F35" s="3" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G35" s="3">
+        <v>4.5</v>
+      </c>
+      <c r="H35" s="3">
+        <v>0.125</v>
+      </c>
+      <c r="I35" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" s="2">
         <v>35</v>
       </c>
@@ -2195,8 +2434,17 @@
       <c r="F36" s="3" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G36" s="3">
+        <v>4.5</v>
+      </c>
+      <c r="H36" s="3">
+        <v>0.125</v>
+      </c>
+      <c r="I36" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" s="2">
         <v>36</v>
       </c>
@@ -2215,8 +2463,17 @@
       <c r="F37" s="3" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G37" s="3">
+        <v>4.5</v>
+      </c>
+      <c r="H37" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="I37" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" s="2">
         <v>37</v>
       </c>
@@ -2235,8 +2492,17 @@
       <c r="F38" s="3" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G38" s="3">
+        <v>4.5</v>
+      </c>
+      <c r="H38" s="3">
+        <v>0.125</v>
+      </c>
+      <c r="I38" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" s="2">
         <v>38</v>
       </c>
@@ -2255,8 +2521,17 @@
       <c r="F39" s="3" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G39" s="3">
+        <v>4.5</v>
+      </c>
+      <c r="H39" s="3">
+        <v>0.125</v>
+      </c>
+      <c r="I39" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" s="2">
         <v>39</v>
       </c>
@@ -2275,8 +2550,17 @@
       <c r="F40" s="3" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G40" s="3">
+        <v>4.5</v>
+      </c>
+      <c r="H40" s="3">
+        <v>0.125</v>
+      </c>
+      <c r="I40" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" s="2">
         <v>40</v>
       </c>
@@ -2295,8 +2579,17 @@
       <c r="F41" s="3" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G41" s="3">
+        <v>4.5</v>
+      </c>
+      <c r="H41" s="3">
+        <v>0.125</v>
+      </c>
+      <c r="I41" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" s="2">
         <v>41</v>
       </c>
@@ -2315,8 +2608,17 @@
       <c r="F42" s="3" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G42" s="3">
+        <v>4.5</v>
+      </c>
+      <c r="H42" s="3">
+        <v>0.125</v>
+      </c>
+      <c r="I42" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" s="2">
         <v>42</v>
       </c>
@@ -2334,13 +2636,23 @@
       </c>
       <c r="F43" s="3" t="s">
         <v>8</v>
+      </c>
+      <c r="G43" s="3">
+        <v>4.5</v>
+      </c>
+      <c r="H43" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="I43" s="3">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="8" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
@@ -3408,7 +3720,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1620EE1C-4891-4E9C-99ED-EB19E309D394}">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
YA DA EL BALANCE DE ENERGÍA
</commit_message>
<xml_diff>
--- a/avances_semanales/fase2/entrada.xlsx
+++ b/avances_semanales/fase2/entrada.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\esteb\Documents\GitHub\analisis_vibraciones\avances_semanales\fase2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{747B69D4-E881-4FB1-8041-F102D2CE7317}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{670CF9DC-4CD8-498E-8222-E78278337B82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="xy_nod" sheetId="1" r:id="rId1"/>
@@ -744,16 +744,6 @@
   </cellStyles>
   <dxfs count="8">
     <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color rgb="FF7F7F7F"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
       <font>
         <b val="0"/>
         <i val="0"/>
@@ -770,6 +760,16 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color rgb="FF7F7F7F"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
       <border outline="0">
@@ -910,7 +910,7 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{96CDDC17-92E8-4C39-B9D1-92DA6FC81046}" name="Table6" displayName="Table6" ref="A1:C3" totalsRowShown="0" headerRowDxfId="2" headerRowCellStyle="Accent2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{96CDDC17-92E8-4C39-B9D1-92DA6FC81046}" name="Table6" displayName="Table6" ref="A1:C3" totalsRowShown="0" headerRowDxfId="0" headerRowCellStyle="Accent2">
   <autoFilter ref="A1:C3" xr:uid="{96CDDC17-92E8-4C39-B9D1-92DA6FC81046}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -934,7 +934,7 @@
   </autoFilter>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{CBB86DB4-091A-4E50-B78A-CE5FA21BDAFD}" name="seccion" dataCellStyle="20% - Accent2"/>
-    <tableColumn id="2" xr3:uid="{79326CC9-9A90-4BFE-99B8-9937ABA40CB9}" name="A" dataDxfId="1" dataCellStyle="Input">
+    <tableColumn id="2" xr3:uid="{79326CC9-9A90-4BFE-99B8-9937ABA40CB9}" name="A" dataDxfId="2" dataCellStyle="Input">
       <calculatedColumnFormula>0.3*0.5</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="3" xr3:uid="{CCC256CD-37B8-4882-BDB5-A78B019F997E}" name="I" dataCellStyle="Input">
@@ -946,7 +946,7 @@
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{20EB72EC-6F79-4D2B-B743-4892BA0EF057}" name="Table8" displayName="Table8" ref="A1:B2651" totalsRowShown="0" tableBorderDxfId="0" headerRowCellStyle="Accent2" dataCellStyle="Input">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{20EB72EC-6F79-4D2B-B743-4892BA0EF057}" name="Table8" displayName="Table8" ref="A1:B2651" totalsRowShown="0" tableBorderDxfId="1" headerRowCellStyle="Accent2" dataCellStyle="Input">
   <autoFilter ref="A1:B2651" xr:uid="{20EB72EC-6F79-4D2B-B743-4892BA0EF057}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -1224,7 +1224,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C29"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
@@ -1323,7 +1323,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="3">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C9" s="3">
         <v>0</v>
@@ -1334,7 +1334,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="3">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C10" s="3">
         <v>3.5</v>
@@ -1345,7 +1345,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="3">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C11" s="3">
         <v>7</v>
@@ -1356,7 +1356,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="3">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C12" s="3">
         <v>10.5</v>
@@ -1367,7 +1367,7 @@
         <v>12</v>
       </c>
       <c r="B13" s="3">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C13" s="3">
         <v>14</v>
@@ -1378,7 +1378,7 @@
         <v>13</v>
       </c>
       <c r="B14" s="3">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C14" s="3">
         <v>17.5</v>
@@ -1389,7 +1389,7 @@
         <v>14</v>
       </c>
       <c r="B15" s="3">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C15" s="3">
         <v>21</v>
@@ -1400,7 +1400,7 @@
         <v>15</v>
       </c>
       <c r="B16" s="3">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C16" s="3">
         <v>0</v>
@@ -1411,7 +1411,7 @@
         <v>16</v>
       </c>
       <c r="B17" s="3">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C17" s="3">
         <v>3.5</v>
@@ -1422,7 +1422,7 @@
         <v>17</v>
       </c>
       <c r="B18" s="3">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C18" s="3">
         <v>7</v>
@@ -1433,7 +1433,7 @@
         <v>18</v>
       </c>
       <c r="B19" s="3">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C19" s="3">
         <v>10.5</v>
@@ -1444,7 +1444,7 @@
         <v>19</v>
       </c>
       <c r="B20" s="3">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C20" s="3">
         <v>14</v>
@@ -1455,7 +1455,7 @@
         <v>20</v>
       </c>
       <c r="B21" s="3">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C21" s="3">
         <v>17.5</v>
@@ -1466,7 +1466,7 @@
         <v>21</v>
       </c>
       <c r="B22" s="3">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C22" s="3">
         <v>21</v>
@@ -1564,7 +1564,7 @@
   <dimension ref="A1:I43"/>
   <sheetViews>
     <sheetView topLeftCell="A19" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="K32" sqref="K32"/>
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3786,7 +3786,7 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection sqref="A1:B1"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3903,7 +3903,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C51B7D3-1B38-4796-965C-F9CD1EA999EB}">
   <dimension ref="A1:B2651"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>

</xml_diff>